<commit_message>
Ich habe mein UML Diagramm für konkrete Sensoren ausgebaut. Außerdem habe ich einen Designbereich erstellt.
</commit_message>
<xml_diff>
--- a/2-Entwurf/Konkrete Bausteine/Sensoren-Einblick.xlsx
+++ b/2-Entwurf/Konkrete Bausteine/Sensoren-Einblick.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEDDD6B-4868-4DF3-AA5B-190253C031EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D0C83A-91E9-4D0D-85DB-CCAC050E2950}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,11 +671,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bausteine - Ich habe in einem UML Diagramm alle möglichen (Bereist in den config-Dateien erwähnten) Attribute für die Sensoren festgehalten.
</commit_message>
<xml_diff>
--- a/2-Entwurf/Konkrete Bausteine/Sensoren-Einblick.xlsx
+++ b/2-Entwurf/Konkrete Bausteine/Sensoren-Einblick.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D0C83A-91E9-4D0D-85DB-CCAC050E2950}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF7EF3D-A517-4BA3-BCCF-C3E9805A4BFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -201,6 +201,13 @@
   </si>
   <si>
     <t>Ermittelt die Distanze zu einem Objekt mittels Timo-of-Flight</t>
+  </si>
+  <si>
+    <t>Digitaler Luftdrucksensor und Temperatursensor</t>
+  </si>
+  <si>
+    <t>Misst Luftdruck
+Auch das Messen von Temperatur ist möglich</t>
   </si>
 </sst>
 </file>
@@ -675,7 +682,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,10 +763,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Ich habe die Dokumentationsstruktur angepasst.
</commit_message>
<xml_diff>
--- a/2-Entwurf/Konkrete Bausteine/Sensoren-Einblick.xlsx
+++ b/2-Entwurf/Konkrete Bausteine/Sensoren-Einblick.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF7EF3D-A517-4BA3-BCCF-C3E9805A4BFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103AA4C2-ED03-4BD6-86D1-3906C8A2A254}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,15 +185,6 @@
     <t>Treiber für die MCP Bauteile</t>
   </si>
   <si>
-    <t>https://www.purelink.de/de/search?sSearch=PS2000</t>
-  </si>
-  <si>
-    <t>HDMI Kabel</t>
-  </si>
-  <si>
-    <t>HDMI Kabel für die entsprechende Datenübertragung</t>
-  </si>
-  <si>
     <t>Distanz-Sensor</t>
   </si>
   <si>
@@ -208,6 +199,15 @@
   <si>
     <t>Misst Luftdruck
 Auch das Messen von Temperatur ist möglich</t>
+  </si>
+  <si>
+    <t>Oszilloskop</t>
+  </si>
+  <si>
+    <t>Stellt Daten dar</t>
+  </si>
+  <si>
+    <t>https://www.picotech.com/oscilloscope/2000/picoscope-2000-overview</t>
   </si>
 </sst>
 </file>
@@ -679,10 +679,10 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,10 +763,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>30</v>
@@ -896,18 +896,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -915,13 +915,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -943,8 +943,8 @@
     <hyperlink ref="D11" r:id="rId15" xr:uid="{312CF08E-319D-4A02-98DE-8475D022F8C1}"/>
     <hyperlink ref="E12" r:id="rId16" xr:uid="{68B80E05-C28F-4E94-B2D2-6CAC80B6E998}"/>
     <hyperlink ref="D13" r:id="rId17" xr:uid="{F7602E41-CEBE-428D-84D3-A3DE38AFE2F3}"/>
-    <hyperlink ref="D14" r:id="rId18" xr:uid="{B37216D5-A8EC-4FA7-8A6F-7BD97B53C3E1}"/>
-    <hyperlink ref="D15" r:id="rId19" xr:uid="{ED251E2B-6437-4699-9AD5-6C7723E21375}"/>
+    <hyperlink ref="D15" r:id="rId18" xr:uid="{ED251E2B-6437-4699-9AD5-6C7723E21375}"/>
+    <hyperlink ref="D14" r:id="rId19" xr:uid="{023A0E55-547F-43A1-9684-D2B1BEA10960}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId20"/>

</xml_diff>